<commit_message>
more grid tiy up
</commit_message>
<xml_diff>
--- a/DataSets/PriceBlotterCommodity.xlsx
+++ b/DataSets/PriceBlotterCommodity.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="31060" windowHeight="11500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26740"/>
   </bookViews>
   <sheets>
     <sheet name="CommodityPrice" sheetId="2" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>Change</t>
   </si>
   <si>
-    <t>PercentChange</t>
-  </si>
-  <si>
     <t>Volume</t>
   </si>
   <si>
@@ -209,12 +206,6 @@
     <t>YearLow</t>
   </si>
   <si>
-    <t>YTDPercentChange</t>
-  </si>
-  <si>
-    <t>OneYearPercentChange</t>
-  </si>
-  <si>
     <t>OTTON</t>
   </si>
   <si>
@@ -234,6 +225,15 @@
   </si>
   <si>
     <t>BidOfferSpread</t>
+  </si>
+  <si>
+    <t>%Change</t>
+  </si>
+  <si>
+    <t>YTD %Change</t>
+  </si>
+  <si>
+    <t>OneYear %Change</t>
   </si>
 </sst>
 </file>
@@ -1048,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1068,13 +1068,13 @@
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -1083,42 +1083,42 @@
         <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -1168,7 +1168,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -1218,7 +1218,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -1268,7 +1268,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -1318,7 +1318,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -1368,10 +1368,10 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>45.54</v>
@@ -1418,10 +1418,10 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <v>46.06</v>
@@ -1468,10 +1468,10 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9">
         <v>2.0939999999999999</v>
@@ -1518,10 +1518,10 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10">
         <v>1.5085999999999999</v>
@@ -1568,10 +1568,10 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11">
         <v>1.3473999999999999</v>
@@ -1618,10 +1618,10 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12">
         <v>1.512</v>
@@ -1654,10 +1654,10 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13">
         <v>27.55</v>
@@ -1684,10 +1684,10 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="5">
         <v>0.43630000000000002</v>
@@ -1714,10 +1714,10 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15">
         <v>465.5</v>
@@ -1764,10 +1764,10 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16">
         <v>379.5</v>
@@ -1814,10 +1814,10 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17">
         <v>15.68</v>
@@ -1864,10 +1864,10 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18">
         <v>1038</v>
@@ -1914,10 +1914,10 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19">
         <v>33.26</v>
@@ -1964,10 +1964,10 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20">
         <v>342.6</v>
@@ -2014,10 +2014,10 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21">
         <v>140.6</v>
@@ -2050,10 +2050,10 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22">
         <v>125.7</v>
@@ -2100,10 +2100,10 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23">
         <v>3076</v>
@@ -2150,10 +2150,10 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24">
         <v>11.244999999999999</v>
@@ -2197,10 +2197,10 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C25">
         <v>194.5</v>
@@ -2247,10 +2247,10 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26">
         <v>12.87</v>
@@ -2289,10 +2289,10 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C27">
         <v>61.77</v>
@@ -2339,10 +2339,10 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28">
         <v>303.89999999999998</v>
@@ -2372,10 +2372,10 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C29">
         <v>120.72499999999999</v>
@@ -2408,10 +2408,10 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30">
         <v>147.17500000000001</v>
@@ -2441,10 +2441,10 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C31">
         <v>81.275000000000006</v>
@@ -2477,10 +2477,10 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32">
         <v>93.88</v>
@@ -2524,10 +2524,10 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C33">
         <v>9275.5</v>
@@ -2574,10 +2574,10 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C34">
         <v>1.4463999999999999</v>
@@ -2624,10 +2624,10 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C35">
         <v>0.73440000000000005</v>
@@ -2674,10 +2674,10 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C36">
         <v>0.77439999999999998</v>
@@ -2724,10 +2724,10 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C37">
         <v>1.0337000000000001</v>
@@ -2774,10 +2774,10 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C38">
         <v>17711</v>
@@ -2821,10 +2821,10 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C39">
         <v>2057.5</v>
@@ -2871,10 +2871,10 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C40">
         <v>4341.25</v>
@@ -2921,10 +2921,10 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C41">
         <v>1454.3</v>
@@ -2971,10 +2971,10 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C42">
         <v>687.9</v>
@@ -3004,10 +3004,10 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C43">
         <v>164.875</v>
@@ -3051,10 +3051,10 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C44">
         <v>109.3984</v>
@@ -3101,10 +3101,10 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C45">
         <v>130.5625</v>
@@ -3151,10 +3151,10 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B46" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C46">
         <v>99.18</v>

</xml_diff>